<commit_message>
쉼표 찍는 코드 추가 common.py, visualization.py
</commit_message>
<xml_diff>
--- a/app/dataset/korea_position.xlsx
+++ b/app/dataset/korea_position.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11203" uniqueCount="3491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12324" uniqueCount="3491">
   <si>
     <t>1단계</t>
   </si>
@@ -10483,14 +10483,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Gyeongsangnam</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gyeongsangbuk</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Gyeonggi</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -10512,6 +10504,14 @@
   </si>
   <si>
     <t>Busan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chungcheongnam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chungcheongbuk</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -10886,8 +10886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3829"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A437" workbookViewId="0">
-      <selection activeCell="A454" sqref="A454"/>
+    <sheetView tabSelected="1" topLeftCell="A2076" workbookViewId="0">
+      <selection activeCell="E2093" sqref="E2093"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -18514,7 +18514,7 @@
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
-        <v>3490</v>
+        <v>3488</v>
       </c>
       <c r="D454">
         <v>129.08000000000001</v>
@@ -18675,7 +18675,7 @@
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
-        <v>3488</v>
+        <v>3486</v>
       </c>
       <c r="B464" t="s">
         <v>24</v>
@@ -18692,7 +18692,7 @@
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
-        <v>3489</v>
+        <v>3487</v>
       </c>
       <c r="B465" t="s">
         <v>465</v>
@@ -30912,7 +30912,7 @@
     </row>
     <row r="1193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1193" t="s">
-        <v>3487</v>
+        <v>3485</v>
       </c>
       <c r="D1193">
         <v>129.31</v>
@@ -31928,7 +31928,7 @@
     </row>
     <row r="1254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1254" t="s">
-        <v>3486</v>
+        <v>3484</v>
       </c>
       <c r="D1254">
         <v>127.29</v>
@@ -32361,7 +32361,7 @@
     </row>
     <row r="1280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1280" t="s">
-        <v>3485</v>
+        <v>3483</v>
       </c>
       <c r="D1280">
         <v>127.01</v>
@@ -43188,7 +43188,7 @@
     </row>
     <row r="1925" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1925" t="s">
-        <v>3484</v>
+        <v>3490</v>
       </c>
       <c r="D1925">
         <v>127.49</v>
@@ -45996,13 +45996,13 @@
     </row>
     <row r="2093" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2093" t="s">
-        <v>3483</v>
+        <v>3489</v>
       </c>
       <c r="D2093">
-        <v>127.42</v>
+        <v>126.8</v>
       </c>
       <c r="E2093">
-        <v>36.32</v>
+        <v>36.51</v>
       </c>
     </row>
     <row r="2094" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>